<commit_message>
Added Panel Accessories Test Data For Spain/Turkey/Hungary market
</commit_message>
<xml_diff>
--- a/Test Data/Gallery_MPM_Attached_Functionality.xlsx
+++ b/Test Data/Gallery_MPM_Attached_Functionality.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A25938-BA9E-4636-9248-3C1ECFBCC68D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFE3F7EE-3B50-4A7B-9384-BC90A8091D7A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="9" xr2:uid="{6166271A-0A48-43E5-8CA4-FA3257AE4873}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="12" xr2:uid="{6166271A-0A48-43E5-8CA4-FA3257AE4873}"/>
   </bookViews>
   <sheets>
     <sheet name="Netherlands" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,9 @@
     <sheet name="Portugal" sheetId="8" r:id="rId8"/>
     <sheet name="Croatia" sheetId="9" r:id="rId9"/>
     <sheet name="Greece" sheetId="10" r:id="rId10"/>
+    <sheet name="Hungary" sheetId="11" r:id="rId11"/>
+    <sheet name="Spain" sheetId="12" r:id="rId12"/>
+    <sheet name="Turkey" sheetId="14" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="48">
   <si>
     <t xml:space="preserve">Note: Do not change the column/rows index </t>
   </si>
@@ -169,6 +172,24 @@
   </si>
   <si>
     <t>NGC-4119/T3169/T3206/T3190</t>
+  </si>
+  <si>
+    <t>Hungary Market</t>
+  </si>
+  <si>
+    <t>NGC-3104/T2998/T2980/T2994</t>
+  </si>
+  <si>
+    <t>Spain Market</t>
+  </si>
+  <si>
+    <t>NGC-3103/T2037/T2051/T2056</t>
+  </si>
+  <si>
+    <t>Turkey Market</t>
+  </si>
+  <si>
+    <t>NGC-3191/T3311/T3317/T3300</t>
   </si>
 </sst>
 </file>
@@ -747,8 +768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB16E29A-EBDF-477C-A88F-4495AD551832}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection sqref="A1:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -793,6 +814,474 @@
       </c>
       <c r="B4" s="3" t="s">
         <v>41</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09FA6EA6-231D-46E4-B389-0F585D5B920F}">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection sqref="A1:D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A29EAEFF-6FEF-4425-8A35-204AD7047E0C}">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection sqref="A1:D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48CE732B-53F7-40B6-860A-7E9AD5A8A2D3}">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="2" t="s">

</xml_diff>

<commit_message>
Added Test Data For Russia/Finland Market
</commit_message>
<xml_diff>
--- a/Test Data/Gallery_MPM_Attached_Functionality.xlsx
+++ b/Test Data/Gallery_MPM_Attached_Functionality.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFE3F7EE-3B50-4A7B-9384-BC90A8091D7A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762D7F72-8683-40C9-9940-5BA81A278AC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="12" xr2:uid="{6166271A-0A48-43E5-8CA4-FA3257AE4873}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="14" xr2:uid="{6166271A-0A48-43E5-8CA4-FA3257AE4873}"/>
   </bookViews>
   <sheets>
     <sheet name="Netherlands" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,8 @@
     <sheet name="Hungary" sheetId="11" r:id="rId11"/>
     <sheet name="Spain" sheetId="12" r:id="rId12"/>
     <sheet name="Turkey" sheetId="14" r:id="rId13"/>
+    <sheet name="Finland" sheetId="15" r:id="rId14"/>
+    <sheet name="Russia" sheetId="16" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="52">
   <si>
     <t xml:space="preserve">Note: Do not change the column/rows index </t>
   </si>
@@ -190,6 +192,18 @@
   </si>
   <si>
     <t>NGC-3191/T3311/T3317/T3300</t>
+  </si>
+  <si>
+    <t>Finland Market</t>
+  </si>
+  <si>
+    <t>NGC-3130/T2949/T2888/T2945</t>
+  </si>
+  <si>
+    <t>Russia Market</t>
+  </si>
+  <si>
+    <t>NGC-2929/T2917/T2911/T2902</t>
   </si>
 </sst>
 </file>
@@ -1235,7 +1249,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48CE732B-53F7-40B6-860A-7E9AD5A8A2D3}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
@@ -1282,6 +1296,318 @@
       </c>
       <c r="B4" s="3" t="s">
         <v>47</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C46E15FB-6D3D-4D05-891B-8426D36B5535}">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18C50D22-751F-40E0-9DD9-B5DDCFC4A1E9}">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="2" t="s">

</xml_diff>